<commit_message>
Save banks data file
</commit_message>
<xml_diff>
--- a/data/processed/banks.xlsx
+++ b/data/processed/banks.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K375"/>
+  <dimension ref="A1:K374"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16471,45 +16471,6 @@
         <v>-10.0545871</v>
       </c>
     </row>
-    <row r="375">
-      <c r="A375" t="n">
-        <v>9.547978248132538e+18</v>
-      </c>
-      <c r="B375" t="inlineStr">
-        <is>
-          <t>Banque Populaire</t>
-        </is>
-      </c>
-      <c r="C375" t="inlineStr">
-        <is>
-          <t>Banque</t>
-        </is>
-      </c>
-      <c r="D375" t="inlineStr">
-        <is>
-          <t>XWVW+35V, Guelmim 81000, MarocXWVW+35V، ڭلميم 81000</t>
-        </is>
-      </c>
-      <c r="E375" t="inlineStr">
-        <is>
-          <t>Guelmim</t>
-        </is>
-      </c>
-      <c r="F375" t="inlineStr"/>
-      <c r="G375" t="n">
-        <v>9</v>
-      </c>
-      <c r="H375" t="n">
-        <v>0</v>
-      </c>
-      <c r="I375" t="inlineStr"/>
-      <c r="J375" t="n">
-        <v>28.9927376</v>
-      </c>
-      <c r="K375" t="n">
-        <v>-10.0545871</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>